<commit_message>
fix decimals in text json
</commit_message>
<xml_diff>
--- a/data_wrangling_2/raw_data/gap_in_ambition.xlsx
+++ b/data_wrangling_2/raw_data/gap_in_ambition.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>126.9542941176471</v>
+        <v>134.8889375</v>
       </c>
     </row>
     <row r="3">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>42.85908571428571</v>
+        <v>50.00226666666666</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>116.5628294117647</v>
+        <v>123.84800625</v>
       </c>
     </row>
     <row r="5">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>14.5964</v>
+        <v>17.02913333333333</v>
       </c>
     </row>
     <row r="6">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>64.01558571428572</v>
+        <v>74.68485</v>
       </c>
     </row>
     <row r="7">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>86.99778823529412</v>
+        <v>92.43515000000001</v>
       </c>
     </row>
     <row r="8">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.02911764705882353</v>
+        <v>0.0309375</v>
       </c>
     </row>
     <row r="10">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3.266142857142857</v>
+        <v>3.8105</v>
       </c>
     </row>
     <row r="11">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.3197058823529412</v>
+        <v>0.3396875</v>
       </c>
     </row>
     <row r="13">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.1229411764705882</v>
+        <v>0.130625</v>
       </c>
     </row>
     <row r="16">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.04305882352941176</v>
+        <v>0.04575</v>
       </c>
     </row>
     <row r="17">
@@ -687,7 +687,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.1868823529411765</v>
+        <v>0.1985625</v>
       </c>
     </row>
     <row r="18">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.01294117647058824</v>
+        <v>0.01375</v>
       </c>
     </row>
     <row r="19">
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0.3005294117647059</v>
+        <v>0.3193125</v>
       </c>
     </row>
     <row r="20">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.08558823529411765</v>
+        <v>0.0909375</v>
       </c>
     </row>
     <row r="21">
@@ -747,7 +747,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0.4829714285714286</v>
+        <v>0.5634666666666667</v>
       </c>
     </row>
     <row r="22">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.2250588235294118</v>
+        <v>0.239125</v>
       </c>
     </row>
     <row r="23">
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>67.71270588235294</v>
+        <v>71.94475</v>
       </c>
     </row>
     <row r="24">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.2351428571428572</v>
+        <v>0.2743333333333334</v>
       </c>
     </row>
     <row r="25">
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.02011764705882353</v>
+        <v>0.021375</v>
       </c>
     </row>
     <row r="27">
@@ -837,7 +837,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>1.065514285714286</v>
+        <v>1.2431</v>
       </c>
     </row>
     <row r="28">
@@ -852,7 +852,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.1711428571428571</v>
+        <v>0.1996666666666667</v>
       </c>
     </row>
     <row r="29">
@@ -882,7 +882,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>0.06258823529411765</v>
+        <v>0.0665</v>
       </c>
     </row>
     <row r="31">
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0.1836</v>
+        <v>0.2142</v>
       </c>
     </row>
     <row r="37">
@@ -987,7 +987,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0.2898571428571429</v>
+        <v>0.3381666666666667</v>
       </c>
     </row>
     <row r="38">
@@ -1017,7 +1017,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>4.928214285714286</v>
+        <v>5.749583333333334</v>
       </c>
     </row>
     <row r="40">
@@ -1047,7 +1047,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0.4121428571428571</v>
+        <v>0.4808333333333333</v>
       </c>
     </row>
     <row r="42">
@@ -1062,7 +1062,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0.003764705882352941</v>
+        <v>0.004</v>
       </c>
     </row>
     <row r="43">
@@ -1077,7 +1077,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0.02582352941176471</v>
+        <v>0.0274375</v>
       </c>
     </row>
     <row r="44">
@@ -1107,7 +1107,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>0.006176470588235295</v>
+        <v>0.006562500000000001</v>
       </c>
     </row>
     <row r="46">
@@ -1122,7 +1122,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0.3594117647058823</v>
+        <v>0.381875</v>
       </c>
     </row>
     <row r="47">
@@ -1137,7 +1137,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0.162</v>
+        <v>0.189</v>
       </c>
     </row>
     <row r="48">
@@ -1152,7 +1152,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>14.12730588235294</v>
+        <v>15.0102625</v>
       </c>
     </row>
     <row r="49">
@@ -1167,7 +1167,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>3.077447058823529</v>
+        <v>3.2697875</v>
       </c>
     </row>
     <row r="50">
@@ -1197,7 +1197,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0.1307142857142857</v>
+        <v>0.1525</v>
       </c>
     </row>
     <row r="52">
@@ -1212,7 +1212,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>0.6178571428571429</v>
+        <v>0.7208333333333333</v>
       </c>
     </row>
     <row r="53">
@@ -1227,7 +1227,7 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>0.8808571428571429</v>
+        <v>1.027666666666667</v>
       </c>
     </row>
     <row r="54">
@@ -1257,7 +1257,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>7.908571428571428</v>
+        <v>9.226666666666667</v>
       </c>
     </row>
     <row r="56">
@@ -1272,7 +1272,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>0.8003529411764706</v>
+        <v>0.850375</v>
       </c>
     </row>
     <row r="57">
@@ -1302,7 +1302,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>0.07588235294117647</v>
+        <v>0.080625</v>
       </c>
     </row>
     <row r="59">
@@ -1317,7 +1317,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>0.0478235294117647</v>
+        <v>0.0508125</v>
       </c>
     </row>
     <row r="60">
@@ -1332,7 +1332,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>0.1104705882352941</v>
+        <v>0.117375</v>
       </c>
     </row>
     <row r="61">
@@ -1362,7 +1362,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>0.007058823529411764</v>
+        <v>0.0075</v>
       </c>
     </row>
     <row r="63">
@@ -1392,7 +1392,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>0.7811764705882352</v>
+        <v>0.83</v>
       </c>
     </row>
     <row r="65">
@@ -1407,7 +1407,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>0.01147058823529412</v>
+        <v>0.0121875</v>
       </c>
     </row>
     <row r="66">
@@ -1422,7 +1422,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>0.7682857142857143</v>
+        <v>0.8963333333333333</v>
       </c>
     </row>
     <row r="67">
@@ -1437,7 +1437,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>0.09411764705882353</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="68">
@@ -1452,7 +1452,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>0.05852941176470589</v>
+        <v>0.0621875</v>
       </c>
     </row>
     <row r="69">
@@ -1467,7 +1467,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>0.01323529411764706</v>
+        <v>0.0140625</v>
       </c>
     </row>
     <row r="70">
@@ -1482,7 +1482,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>0.2407058823529412</v>
+        <v>0.25575</v>
       </c>
     </row>
     <row r="71">
@@ -1512,7 +1512,7 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>0.01117647058823529</v>
+        <v>0.011875</v>
       </c>
     </row>
     <row r="73">
@@ -1527,7 +1527,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>0.007058823529411764</v>
+        <v>0.0075</v>
       </c>
     </row>
     <row r="74">
@@ -1542,7 +1542,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>0.5</v>
+        <v>0.5833333333333334</v>
       </c>
     </row>
     <row r="75">
@@ -1557,7 +1557,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>0.02176470588235294</v>
+        <v>0.023125</v>
       </c>
     </row>
     <row r="76">
@@ -1572,7 +1572,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>0.1071428571428571</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="77">
@@ -1602,7 +1602,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>0.01673529411764706</v>
+        <v>0.01778125</v>
       </c>
     </row>
     <row r="79">
@@ -1617,7 +1617,7 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>0.2176470588235294</v>
+        <v>0.23125</v>
       </c>
     </row>
     <row r="80">
@@ -1632,7 +1632,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>0.04847058823529412</v>
+        <v>0.0515</v>
       </c>
     </row>
     <row r="81">
@@ -1662,7 +1662,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>0.4581176470588235</v>
+        <v>0.48675</v>
       </c>
     </row>
     <row r="83">
@@ -1677,7 +1677,7 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>0.018</v>
+        <v>0.019125</v>
       </c>
     </row>
     <row r="84">
@@ -1722,7 +1722,7 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>0.7195529411764706</v>
+        <v>0.764525</v>
       </c>
     </row>
     <row r="87">
@@ -1737,7 +1737,7 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>4.065285714285714</v>
+        <v>4.742833333333333</v>
       </c>
     </row>
     <row r="88">
@@ -1767,7 +1767,7 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>0.1738235294117647</v>
+        <v>0.1846875</v>
       </c>
     </row>
     <row r="90">
@@ -1782,7 +1782,7 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>2.224182352941177</v>
+        <v>2.36319375</v>
       </c>
     </row>
     <row r="91">
@@ -1810,7 +1810,7 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>0.009117647058823529</v>
+        <v>0.0096875</v>
       </c>
     </row>
     <row r="93">
@@ -1825,7 +1825,7 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>0.2627647058823529</v>
+        <v>0.2791875</v>
       </c>
     </row>
     <row r="94">
@@ -1840,7 +1840,7 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>0.03914285714285715</v>
+        <v>0.04566666666666667</v>
       </c>
     </row>
     <row r="95">
@@ -1855,7 +1855,7 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>0.1527142857142857</v>
+        <v>0.1781666666666667</v>
       </c>
     </row>
     <row r="96">
@@ -1870,7 +1870,7 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>2.746711764705882</v>
+        <v>2.91838125</v>
       </c>
     </row>
     <row r="97">
@@ -1885,7 +1885,7 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>5.883428571428571</v>
+        <v>6.864</v>
       </c>
     </row>
     <row r="98">
@@ -1900,7 +1900,7 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>0.4143571428571429</v>
+        <v>0.4834166666666667</v>
       </c>
     </row>
     <row r="99">
@@ -1915,7 +1915,7 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>0.05294117647058823</v>
+        <v>0.05624999999999999</v>
       </c>
     </row>
     <row r="100">
@@ -1960,7 +1960,7 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>0.003529411764705882</v>
+        <v>0.00375</v>
       </c>
     </row>
     <row r="103">
@@ -1975,7 +1975,7 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>1.126823529411765</v>
+        <v>1.19725</v>
       </c>
     </row>
     <row r="104">
@@ -1990,7 +1990,7 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>0.02352941176470588</v>
+        <v>0.025</v>
       </c>
     </row>
     <row r="105">
@@ -2020,7 +2020,7 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>0.3610588235294118</v>
+        <v>0.383625</v>
       </c>
     </row>
     <row r="107">
@@ -2035,7 +2035,7 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>2.981885714285714</v>
+        <v>3.478866666666667</v>
       </c>
     </row>
     <row r="108">
@@ -2050,7 +2050,7 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>1.263352941176471</v>
+        <v>1.3423125</v>
       </c>
     </row>
     <row r="109">
@@ -2080,7 +2080,7 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>0.3102857142857143</v>
+        <v>0.362</v>
       </c>
     </row>
     <row r="111">
@@ -2095,7 +2095,7 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>28.05832857142857</v>
+        <v>32.73471666666666</v>
       </c>
     </row>
     <row r="112">
@@ -2110,7 +2110,7 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>0.1466470588235294</v>
+        <v>0.1558125</v>
       </c>
     </row>
     <row r="113">
@@ -2140,7 +2140,7 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>1.602294117647059</v>
+        <v>1.7024375</v>
       </c>
     </row>
     <row r="115">
@@ -2155,7 +2155,7 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>0.01941176470588235</v>
+        <v>0.020625</v>
       </c>
     </row>
     <row r="116">
@@ -2170,7 +2170,7 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>0.09823529411764707</v>
+        <v>0.104375</v>
       </c>
     </row>
     <row r="117">
@@ -2185,7 +2185,7 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>18.56011176470588</v>
+        <v>18.83569375</v>
       </c>
     </row>
     <row r="118">
@@ -2200,7 +2200,7 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>22.90035714285714</v>
+        <v>17.56473333333333</v>
       </c>
     </row>
     <row r="119">
@@ -2215,7 +2215,7 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>16.35422941176471</v>
+        <v>16.54975625</v>
       </c>
     </row>
     <row r="120">
@@ -2230,7 +2230,7 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>9.672557142857142</v>
+        <v>7.7516</v>
       </c>
     </row>
     <row r="121">
@@ -2245,7 +2245,7 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>33.6457</v>
+        <v>24.23241666666667</v>
       </c>
     </row>
     <row r="122">
@@ -2260,7 +2260,7 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>2.520823529411765</v>
+        <v>2.621125</v>
       </c>
     </row>
     <row r="123">
@@ -2290,7 +2290,7 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>0.02205882352941177</v>
+        <v>0.0234375</v>
       </c>
     </row>
     <row r="125">
@@ -2305,7 +2305,7 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>2.590428571428572</v>
+        <v>1.010666666666667</v>
       </c>
     </row>
     <row r="126">
@@ -2380,7 +2380,7 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>0.02470588235294117</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="131">
@@ -2395,7 +2395,7 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>0.007764705882352942</v>
+        <v>0.00825</v>
       </c>
     </row>
     <row r="132">
@@ -2410,7 +2410,7 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>0.146</v>
+        <v>0.150375</v>
       </c>
     </row>
     <row r="133">
@@ -2470,7 +2470,7 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>0.4672571428571429</v>
+        <v>0.4951333333333334</v>
       </c>
     </row>
     <row r="137">
@@ -2485,7 +2485,7 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>0.2250588235294118</v>
+        <v>0.21825</v>
       </c>
     </row>
     <row r="138">
@@ -2500,7 +2500,7 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>0.3100000000000001</v>
+        <v>0.28625</v>
       </c>
     </row>
     <row r="139">
@@ -2515,7 +2515,7 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>0.08371428571428571</v>
+        <v>0.03933333333333334</v>
       </c>
     </row>
     <row r="140">
@@ -2560,7 +2560,7 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>0.1895714285714286</v>
+        <v>0.2211666666666667</v>
       </c>
     </row>
     <row r="143">
@@ -2575,7 +2575,7 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>0.1711428571428571</v>
+        <v>0.06849999999999999</v>
       </c>
     </row>
     <row r="144">
@@ -2695,7 +2695,7 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>0.178</v>
+        <v>0.2076666666666667</v>
       </c>
     </row>
     <row r="152">
@@ -2710,7 +2710,7 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>0.2898571428571429</v>
+        <v>0.3178333333333334</v>
       </c>
     </row>
     <row r="153">
@@ -2740,7 +2740,7 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>3.842071428571429</v>
+        <v>2.739416666666667</v>
       </c>
     </row>
     <row r="155">
@@ -2770,7 +2770,7 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>0.4121428571428572</v>
+        <v>0.4808333333333334</v>
       </c>
     </row>
     <row r="157">
@@ -2830,7 +2830,7 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>0.006176470588235295</v>
+        <v>0.006562500000000001</v>
       </c>
     </row>
     <row r="161">
@@ -2860,7 +2860,7 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>0.1434285714285714</v>
+        <v>0.1473333333333333</v>
       </c>
     </row>
     <row r="163">
@@ -2875,7 +2875,7 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>0.02470588235294117</v>
+        <v>0.02625</v>
       </c>
     </row>
     <row r="164">
@@ -2890,7 +2890,7 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>0.1193529411764706</v>
+        <v>0.1190625</v>
       </c>
     </row>
     <row r="165">
@@ -2920,7 +2920,7 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>0.1307142857142857</v>
+        <v>0.1525</v>
       </c>
     </row>
     <row r="167">
@@ -2935,7 +2935,7 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>0.6178571428571429</v>
+        <v>0.7208333333333333</v>
       </c>
     </row>
     <row r="168">
@@ -2950,7 +2950,7 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>0.8808571428571429</v>
+        <v>0.9716666666666667</v>
       </c>
     </row>
     <row r="169">
@@ -2980,7 +2980,7 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>0.6752571428571429</v>
+        <v>0.2361333333333333</v>
       </c>
     </row>
     <row r="171">
@@ -2995,7 +2995,7 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>0.07488235294117648</v>
+        <v>0.0733125</v>
       </c>
     </row>
     <row r="172">
@@ -3025,7 +3025,7 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>0.02411764705882353</v>
+        <v>0.025625</v>
       </c>
     </row>
     <row r="174">
@@ -3040,7 +3040,7 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>0.03017647058823529</v>
+        <v>0.0320625</v>
       </c>
     </row>
     <row r="175">
@@ -3115,7 +3115,7 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>0.4358823529411764</v>
+        <v>0.463125</v>
       </c>
     </row>
     <row r="180">
@@ -3145,7 +3145,7 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>0.2</v>
+        <v>0.2333333333333333</v>
       </c>
     </row>
     <row r="182">
@@ -3190,7 +3190,7 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>0.01323529411764706</v>
+        <v>0.0140625</v>
       </c>
     </row>
     <row r="185">
@@ -3250,7 +3250,7 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>0.007058823529411764</v>
+        <v>0.0075</v>
       </c>
     </row>
     <row r="189">
@@ -3265,7 +3265,7 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>0.5</v>
+        <v>0.5833333333333334</v>
       </c>
     </row>
     <row r="190">
@@ -3280,7 +3280,7 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>0.005882352941176471</v>
+        <v>0.00625</v>
       </c>
     </row>
     <row r="191">
@@ -3295,7 +3295,7 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>0.1071428571428571</v>
+        <v>0</v>
       </c>
     </row>
     <row r="192">
@@ -3355,7 +3355,7 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>0.04847058823529412</v>
+        <v>0.0515</v>
       </c>
     </row>
     <row r="196">
@@ -3400,7 +3400,7 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>0.018</v>
+        <v>0.019125</v>
       </c>
     </row>
     <row r="199">
@@ -3445,7 +3445,7 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>0.02952941176470588</v>
+        <v>0.031375</v>
       </c>
     </row>
     <row r="202">
@@ -3460,7 +3460,7 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>2.135985714285714</v>
+        <v>1.246816666666667</v>
       </c>
     </row>
     <row r="203">
@@ -3490,7 +3490,7 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>0.1708823529411765</v>
+        <v>0.1815625</v>
       </c>
     </row>
     <row r="205">
@@ -3505,7 +3505,7 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>0.2455882352941176</v>
+        <v>0.2515625</v>
       </c>
     </row>
     <row r="206">
@@ -3548,7 +3548,7 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>0.06594117647058824</v>
+        <v>0.045625</v>
       </c>
     </row>
     <row r="209">
@@ -3563,7 +3563,7 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>0.009428571428571429</v>
+        <v>0.011</v>
       </c>
     </row>
     <row r="210">
@@ -3578,7 +3578,7 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>0.1455714285714286</v>
+        <v>0</v>
       </c>
     </row>
     <row r="211">
@@ -3593,7 +3593,7 @@
         </is>
       </c>
       <c r="C211" t="n">
-        <v>1.794529411764706</v>
+        <v>1.9066875</v>
       </c>
     </row>
     <row r="212">
@@ -3608,7 +3608,7 @@
         </is>
       </c>
       <c r="C212" t="n">
-        <v>2.837142857142857</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="213">
@@ -3623,7 +3623,7 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>0.2287857142857143</v>
+        <v>0.1443666666666667</v>
       </c>
     </row>
     <row r="214">
@@ -3698,7 +3698,7 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>0.6448823529411766</v>
+        <v>0.6851875000000001</v>
       </c>
     </row>
     <row r="219">
@@ -3743,7 +3743,7 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>0.2111176470588235</v>
+        <v>0.2243125</v>
       </c>
     </row>
     <row r="222">
@@ -3758,7 +3758,7 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>0.06428571428571428</v>
+        <v>0</v>
       </c>
     </row>
     <row r="223">
@@ -3803,7 +3803,7 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>0.3102857142857143</v>
+        <v>0</v>
       </c>
     </row>
     <row r="226">
@@ -3818,7 +3818,7 @@
         </is>
       </c>
       <c r="C226" t="n">
-        <v>16.43477142857143</v>
+        <v>12.80455</v>
       </c>
     </row>
     <row r="227">

</xml_diff>